<commit_message>
added table with squares
</commit_message>
<xml_diff>
--- a/check_list.xlsx
+++ b/check_list.xlsx
@@ -1,136 +1,136 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20337"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20337"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gleb Onore\Documents\VDK\ror-tool_seed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B77D60F-6685-4CC9-92BE-FC86209A6148}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EAE758-4F14-4718-B4D5-5173AB97085C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
   <si>
+    <t>Дата</t>
+  </si>
+  <si>
+    <t>ФИО лаборанта</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Время </t>
+  </si>
+  <si>
+    <t>Место отбора</t>
+  </si>
+  <si>
+    <t>ПШЕНИЦА</t>
+  </si>
+  <si>
+    <t>Класс</t>
+  </si>
+  <si>
     <t>Влажность, %</t>
   </si>
   <si>
+    <t>FOSS</t>
+  </si>
+  <si>
+    <t>A&amp;D</t>
+  </si>
+  <si>
+    <t>СЭШ</t>
+  </si>
+  <si>
     <t>Протеин, FOSS</t>
   </si>
   <si>
+    <t>Клейковина,%</t>
+  </si>
+  <si>
     <t>Протеин, % хім</t>
   </si>
   <si>
+    <t>ИДК, у.е.</t>
+  </si>
+  <si>
     <t>Клейковина, % FOSS</t>
   </si>
   <si>
+    <t>Натура, г/л</t>
+  </si>
+  <si>
     <t>ЧП, сек</t>
   </si>
   <si>
+    <t>Заражен</t>
+  </si>
+  <si>
     <t>м пробы</t>
   </si>
   <si>
+    <t>г</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Запах/цвет</t>
+  </si>
+  <si>
     <t>м навески</t>
   </si>
   <si>
+    <t>М 1000зер.</t>
+  </si>
+  <si>
     <t>круп.сорт</t>
   </si>
   <si>
+    <t>Зер. повр.клоп/ч</t>
+  </si>
+  <si>
     <t>минер.пр</t>
   </si>
   <si>
+    <t>битые</t>
+  </si>
+  <si>
     <t>орган.пр</t>
   </si>
   <si>
+    <t>щуплые</t>
+  </si>
+  <si>
     <t>сор.сем</t>
   </si>
   <si>
+    <t>проросшие</t>
+  </si>
+  <si>
     <t>др. культуры</t>
   </si>
   <si>
-    <t>битые</t>
-  </si>
-  <si>
-    <t>проросшие</t>
-  </si>
-  <si>
     <t>изъеденные</t>
   </si>
   <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>Дата</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Время </t>
-  </si>
-  <si>
-    <t>ФИО лаборанта</t>
-  </si>
-  <si>
-    <t>Место отбора</t>
-  </si>
-  <si>
-    <t>ПШЕНИЦА</t>
-  </si>
-  <si>
-    <t>FOSS</t>
-  </si>
-  <si>
-    <t>г</t>
+    <t>др. культуры:</t>
   </si>
   <si>
     <t>СОР.ПРИМ.</t>
   </si>
   <si>
-    <t>A&amp;D</t>
-  </si>
-  <si>
-    <t>СЭШ</t>
-  </si>
-  <si>
-    <t>Клейковина,%</t>
-  </si>
-  <si>
-    <t>ИДК, у.е.</t>
-  </si>
-  <si>
-    <t>Натура, г/л</t>
-  </si>
-  <si>
-    <t>Заражен</t>
-  </si>
-  <si>
-    <t>Запах/цвет</t>
-  </si>
-  <si>
     <t>ЗЕРН. ПРИМ.</t>
-  </si>
-  <si>
-    <t>Класс</t>
-  </si>
-  <si>
-    <t>М 1000зер.</t>
-  </si>
-  <si>
-    <t>Зер. повр.клоп/ч</t>
-  </si>
-  <si>
-    <t>щуплые</t>
-  </si>
-  <si>
-    <t>др. культуры:</t>
   </si>
 </sst>
 </file>
@@ -163,7 +163,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -186,11 +186,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -199,6 +212,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -540,7 +554,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,26 +568,26 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -583,278 +597,278 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -863,11 +877,11 @@
   <mergeCells count="5">
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F9:G9"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix plot's update; add nwe version modelsweight.pt
</commit_message>
<xml_diff>
--- a/check_list.xlsx
+++ b/check_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gleb Onore\Documents\VDK\ror-tool_seed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EAE758-4F14-4718-B4D5-5173AB97085C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C5DFE2-1655-4714-8EB7-CEFD830C2B5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>Дата</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>ЗЕРН. ПРИМ.</t>
+  </si>
+  <si>
+    <t>ячмень</t>
   </si>
 </sst>
 </file>
@@ -554,7 +557,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -835,7 +838,9 @@
         <v>20</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="F17" s="2" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
fix plot's update; add new version modelsweight.pt
</commit_message>
<xml_diff>
--- a/check_list.xlsx
+++ b/check_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gleb Onore\Documents\VDK\ror-tool_seed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C5DFE2-1655-4714-8EB7-CEFD830C2B5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CCF709-8969-497F-9C95-ADCC605B960E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>Дата</t>
   </si>
@@ -118,9 +118,6 @@
     <t>проросшие</t>
   </si>
   <si>
-    <t>др. культуры</t>
-  </si>
-  <si>
     <t>изъеденные</t>
   </si>
   <si>
@@ -134,6 +131,9 @@
   </si>
   <si>
     <t>ячмень</t>
+  </si>
+  <si>
+    <t>овсюг</t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,17 +791,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>19</v>
@@ -811,7 +807,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
@@ -820,14 +818,10 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
@@ -839,7 +833,7 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>19</v>
@@ -867,13 +861,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>

</xml_diff>